<commit_message>
penultimate revisions including powerpoint, pdf, and code organization
</commit_message>
<xml_diff>
--- a/directors.xlsx
+++ b/directors.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamailman/Desktop/Metis_Bootcamp/Metis_Bootcamp_repos/scrape_flix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E0B251-CE12-3742-9D04-FF00C9F14531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13A5476-4D9C-C147-97B7-00535A7DDC9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7660" yWindow="460" windowWidth="18980" windowHeight="14100" activeTab="1" xr2:uid="{430FB6C8-4E99-2C4C-88D9-584E09F63679}"/>
+    <workbookView xWindow="5420" yWindow="460" windowWidth="23680" windowHeight="13920" activeTab="1" xr2:uid="{430FB6C8-4E99-2C4C-88D9-584E09F63679}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="poly" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet1!$A$1:$I$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet1!$A$1:$I$10</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t>Hitchcock</t>
   </si>
@@ -107,34 +107,6 @@
         <color theme="1"/>
         <rFont val="Montserrat"/>
       </rPr>
-      <t xml:space="preserve">Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">&amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Ratings count</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
       <t>Year</t>
     </r>
     <r>
@@ -251,9 +223,6 @@
     <t>Lasso CV</t>
   </si>
   <si>
-    <t>r2</t>
-  </si>
-  <si>
     <t>w/ rating count</t>
   </si>
   <si>
@@ -319,15 +288,57 @@
       <t xml:space="preserve"> logs</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Rating count</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat Regular"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,6 +466,18 @@
       <color rgb="FF00B050"/>
       <name val="Montserrat Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Montserrat Regular"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Montserrat Regular"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -464,7 +487,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -544,8 +567,30 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -557,8 +602,17 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -649,26 +703,35 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,118 +1045,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3D6B10-E7B3-9142-A566-3C95F796046B}">
-  <dimension ref="A10:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5011BA73-3AD7-E143-BE9C-8A47C978D16E}">
+  <dimension ref="A8:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="27"/>
-    <col min="2" max="2" width="21.1640625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="27" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="27"/>
     <col min="4" max="10" width="11.83203125" style="27" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
+    <row r="8" spans="1:11">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+    </row>
     <row r="10" spans="1:11">
       <c r="A10" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="39" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="18">
       <c r="A11" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D11" s="34">
-        <v>0.79790000000000005</v>
+        <v>0.76946000000000003</v>
       </c>
       <c r="E11" s="34">
-        <v>0.47370000000000001</v>
+        <v>0.27210000000000001</v>
       </c>
       <c r="F11" s="34">
-        <v>-2.46E-2</v>
+        <v>8.9300000000000004E-2</v>
       </c>
       <c r="G11" s="34">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="H11" s="34">
-        <v>9.6799999999999997E-2</v>
+        <v>-0.47960000000000003</v>
+      </c>
+      <c r="H11" s="54">
+        <v>0.28039999999999998</v>
       </c>
       <c r="I11" s="34">
-        <v>0.29470000000000002</v>
+        <v>0.2571</v>
       </c>
       <c r="J11" s="34">
-        <v>0.33689999999999998</v>
+        <v>-1.6642999999999999</v>
       </c>
       <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11">
       <c r="C12" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="33">
-        <v>0.307</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="32">
+        <v>0.32967000000000002</v>
       </c>
       <c r="E12" s="32">
-        <v>0.47949999999999998</v>
+        <v>0.53120000000000001</v>
       </c>
       <c r="F12" s="32">
-        <v>0.48630000000000001</v>
+        <v>0.48643999999999998</v>
       </c>
       <c r="G12" s="32">
-        <v>0.3856</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="H12" s="32">
-        <v>0.57869999999999999</v>
+        <v>0.55259999999999998</v>
       </c>
       <c r="I12" s="32">
-        <v>0.36059999999999998</v>
+        <v>0.34639999999999999</v>
       </c>
       <c r="J12" s="32">
-        <v>0.3049</v>
+        <v>0.3483</v>
       </c>
       <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="D13" s="33"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
       <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -1104,30 +1179,30 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" ht="18">
       <c r="A15" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D15" s="34">
-        <v>0.14599999999999999</v>
+        <v>9.5530000000000004E-2</v>
       </c>
       <c r="E15" s="34">
-        <v>4.9299999999999997E-2</v>
-      </c>
-      <c r="F15" s="45">
-        <v>7.5600000000000001E-2</v>
+        <v>5.2150000000000002E-2</v>
+      </c>
+      <c r="F15" s="42">
+        <v>-0.30809999999999998</v>
       </c>
       <c r="G15" s="34">
-        <v>-0.33177000000000001</v>
-      </c>
-      <c r="H15" s="34">
-        <v>-3.4299999999999997E-2</v>
-      </c>
-      <c r="I15" s="44">
-        <v>0.18379999999999999</v>
+        <v>-0.59399999999999997</v>
+      </c>
+      <c r="H15" s="46">
+        <v>0.20860000000000001</v>
+      </c>
+      <c r="I15" s="46">
+        <v>0.1925</v>
       </c>
       <c r="J15" s="34">
         <v>-6.8699999999999997E-2</v>
@@ -1136,89 +1211,89 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" s="34">
-        <v>0.38059999999999999</v>
+        <v>0.32854</v>
       </c>
       <c r="E16" s="36">
-        <v>0.20710000000000001</v>
+        <v>0.45650000000000002</v>
       </c>
       <c r="F16" s="34">
-        <v>-0.14949999999999999</v>
+        <v>-6.8999999999999999E-3</v>
       </c>
       <c r="G16" s="34">
-        <v>-0.21229999999999999</v>
-      </c>
-      <c r="H16" s="44">
-        <v>7.2599999999999998E-2</v>
+        <v>-0.28089999999999998</v>
+      </c>
+      <c r="H16" s="42">
+        <v>0.12820000000000001</v>
       </c>
       <c r="I16" s="34">
-        <v>0.107</v>
+        <v>-0.13730000000000001</v>
       </c>
       <c r="J16" s="34">
-        <v>-5.2699999999999997E-2</v>
+        <v>-1.3768</v>
       </c>
       <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="33">
-        <v>0.59089999999999998</v>
-      </c>
-      <c r="E17" s="32">
-        <v>0.69810000000000005</v>
+        <v>25</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.62385999999999997</v>
+      </c>
+      <c r="E17" s="45">
+        <v>0.69257999999999997</v>
       </c>
       <c r="F17" s="32">
-        <v>0.47220000000000001</v>
+        <v>0.50719000000000003</v>
       </c>
       <c r="G17" s="32">
-        <v>0.42109999999999997</v>
+        <v>0.51219999999999999</v>
       </c>
       <c r="H17" s="32">
-        <v>0.64970000000000006</v>
-      </c>
-      <c r="I17" s="42">
-        <v>0.39040000000000002</v>
-      </c>
-      <c r="J17" s="41">
-        <v>0.35049999999999998</v>
+        <v>0.64149999999999996</v>
+      </c>
+      <c r="I17" s="45">
+        <v>0.38590000000000002</v>
+      </c>
+      <c r="J17" s="45">
+        <v>0.35849999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="39">
-        <v>0.50970000000000004</v>
-      </c>
-      <c r="E18" s="43">
-        <v>0.61380000000000001</v>
+        <v>24</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.4904</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0.51519999999999999</v>
       </c>
       <c r="F18" s="32">
-        <v>0.50229999999999997</v>
+        <v>0.47670000000000001</v>
       </c>
       <c r="G18" s="32">
-        <v>0.4375</v>
+        <v>0.44940000000000002</v>
       </c>
       <c r="H18" s="32">
-        <v>0.63249999999999995</v>
-      </c>
-      <c r="I18" s="42">
-        <v>0.34889999999999999</v>
-      </c>
-      <c r="J18" s="32">
-        <v>0.37090000000000001</v>
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="I18" s="44">
+        <v>0.3826</v>
+      </c>
+      <c r="J18" s="44">
+        <v>0.55600000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="35"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
@@ -1228,7 +1303,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
@@ -1238,122 +1313,494 @@
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="18">
       <c r="A21" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D21" s="36">
-        <v>0.2442</v>
+        <v>0.29054000000000002</v>
       </c>
       <c r="E21" s="34">
-        <v>-0.3382</v>
-      </c>
-      <c r="F21" s="34">
-        <v>0.1542</v>
+        <v>-0.47789999999999999</v>
+      </c>
+      <c r="F21" s="54">
+        <v>0.37680000000000002</v>
       </c>
       <c r="G21" s="34">
         <v>-0.1116</v>
       </c>
       <c r="I21" s="34">
-        <v>-1.2285999999999999</v>
+        <v>-1.3102</v>
       </c>
       <c r="J21" s="34">
-        <v>-0.2586</v>
+        <v>-4.0671999999999997</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D22" s="34">
-        <v>0.22639999999999999</v>
+        <v>0.10009</v>
       </c>
       <c r="E22" s="34">
-        <v>-0.71830000000000005</v>
+        <v>-0.19635</v>
       </c>
       <c r="F22" s="34">
-        <v>-6.93E-2</v>
+        <v>-0.1767</v>
       </c>
       <c r="G22" s="34">
-        <v>-2.69E-2</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>29</v>
+        <v>-0.65239999999999998</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="I22" s="34">
-        <v>-1.38842</v>
+        <v>-1.9036</v>
       </c>
       <c r="J22" s="34">
-        <v>-0.14299999999999999</v>
+        <v>-0.62970000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="40">
-        <v>0.39929999999999999</v>
+        <v>25</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0.38616</v>
       </c>
       <c r="E23" s="32">
-        <v>0.75</v>
-      </c>
-      <c r="F23" s="32">
-        <v>0.46079999999999999</v>
-      </c>
-      <c r="G23" s="32">
+        <v>0.84240000000000004</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0.3952</v>
+      </c>
+      <c r="G23" s="49">
         <v>0.35499999999999998</v>
       </c>
-      <c r="H23" s="47" t="s">
-        <v>30</v>
+      <c r="H23" s="40" t="s">
+        <v>28</v>
       </c>
       <c r="I23" s="32">
         <v>0.45179999999999998</v>
       </c>
       <c r="J23" s="32">
-        <v>0.52100000000000002</v>
+        <v>0.99109999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="33">
-        <v>0.41349999999999998</v>
-      </c>
-      <c r="E24" s="32">
-        <v>0.82550000000000001</v>
-      </c>
-      <c r="F24" s="38">
-        <v>0.37169999999999997</v>
-      </c>
-      <c r="G24" s="38">
-        <v>0.32790000000000002</v>
+        <v>24</v>
+      </c>
+      <c r="D24" s="44">
+        <v>0.42886999999999997</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0.92811999999999995</v>
+      </c>
+      <c r="F24" s="44">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="G24" s="50">
+        <v>0.4118</v>
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="32">
-        <v>0.45529999999999998</v>
+        <v>0.44259999999999999</v>
       </c>
       <c r="J24" s="32">
-        <v>0.56899999999999995</v>
+        <v>0.66269999999999996</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3D6B10-E7B3-9142-A566-3C95F796046B}">
+  <dimension ref="A10:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="27"/>
+    <col min="2" max="2" width="13.83203125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="27"/>
+    <col min="4" max="10" width="11.83203125" style="27" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="1:11">
+      <c r="A10" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="18">
+      <c r="A11" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="54">
+        <v>0.79790000000000005</v>
+      </c>
+      <c r="E11" s="54">
+        <v>0.47370000000000001</v>
+      </c>
+      <c r="F11" s="34">
+        <v>-2.46E-2</v>
+      </c>
+      <c r="G11" s="54">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H11" s="34">
+        <v>9.6799999999999997E-2</v>
+      </c>
+      <c r="I11" s="54">
+        <v>0.29470000000000002</v>
+      </c>
+      <c r="J11" s="54">
+        <v>0.33689999999999998</v>
+      </c>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.307</v>
+      </c>
+      <c r="E12" s="32">
+        <v>0.47949999999999998</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0.48630000000000001</v>
+      </c>
+      <c r="G12" s="32">
+        <v>0.3856</v>
+      </c>
+      <c r="H12" s="32">
+        <v>0.57869999999999999</v>
+      </c>
+      <c r="I12" s="32">
+        <v>0.36059999999999998</v>
+      </c>
+      <c r="J12" s="32">
+        <v>0.3049</v>
+      </c>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+    </row>
+    <row r="15" spans="1:11" ht="18">
+      <c r="A15" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="34">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="E15" s="34">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="F15" s="42">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="G15" s="34">
+        <v>-0.33177000000000001</v>
+      </c>
+      <c r="H15" s="34">
+        <v>-3.4299999999999997E-2</v>
+      </c>
+      <c r="I15" s="46">
+        <v>0.18379999999999999</v>
+      </c>
+      <c r="J15" s="34">
+        <v>-6.8699999999999997E-2</v>
+      </c>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0.38059999999999999</v>
+      </c>
+      <c r="E16" s="36">
+        <v>0.20710000000000001</v>
+      </c>
+      <c r="F16" s="42">
+        <v>-0.14949999999999999</v>
+      </c>
+      <c r="G16" s="34">
+        <v>-0.21229999999999999</v>
+      </c>
+      <c r="H16" s="46">
+        <v>7.2599999999999998E-2</v>
+      </c>
+      <c r="I16" s="42">
+        <v>0.107</v>
+      </c>
+      <c r="J16" s="34">
+        <v>-5.2699999999999997E-2</v>
+      </c>
+      <c r="K16" s="32"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="32">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="E17" s="45">
+        <v>0.69810000000000005</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0.47220000000000001</v>
+      </c>
+      <c r="G17" s="32">
+        <v>0.42109999999999997</v>
+      </c>
+      <c r="H17" s="32">
+        <v>0.64970000000000006</v>
+      </c>
+      <c r="I17" s="45">
+        <v>0.39040000000000002</v>
+      </c>
+      <c r="J17" s="49">
+        <v>0.35049999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="32">
+        <v>0.50970000000000004</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0.61380000000000001</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="G18" s="32">
+        <v>0.4375</v>
+      </c>
+      <c r="H18" s="32">
+        <v>0.63249999999999995</v>
+      </c>
+      <c r="I18" s="44">
+        <v>0.34889999999999999</v>
+      </c>
+      <c r="J18" s="50">
+        <v>0.37090000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="35"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:10" ht="18">
+      <c r="A21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="36">
+        <v>0.2442</v>
+      </c>
+      <c r="E21" s="34">
+        <v>-0.3382</v>
+      </c>
+      <c r="F21" s="36">
+        <v>0.1542</v>
+      </c>
+      <c r="G21" s="34">
+        <v>-0.1116</v>
+      </c>
+      <c r="I21" s="34">
+        <v>-1.2285999999999999</v>
+      </c>
+      <c r="J21" s="34">
+        <v>-0.2586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="34">
+        <v>0.22639999999999999</v>
+      </c>
+      <c r="E22" s="34">
+        <v>-0.71830000000000005</v>
+      </c>
+      <c r="F22" s="34">
+        <v>-6.93E-2</v>
+      </c>
+      <c r="G22" s="34">
+        <v>-2.69E-2</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="34">
+        <v>-1.38842</v>
+      </c>
+      <c r="J22" s="34">
+        <v>-0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0.39929999999999999</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0.75</v>
+      </c>
+      <c r="F23" s="47">
+        <v>0.46079999999999999</v>
+      </c>
+      <c r="G23" s="45">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="32">
+        <v>0.45179999999999998</v>
+      </c>
+      <c r="J23" s="32">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="44">
+        <v>0.41349999999999998</v>
+      </c>
+      <c r="E24" s="32">
+        <v>0.82550000000000001</v>
+      </c>
+      <c r="F24" s="48">
+        <v>0.37169999999999997</v>
+      </c>
+      <c r="G24" s="44">
+        <v>0.32790000000000002</v>
+      </c>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32">
+        <v>0.45529999999999998</v>
+      </c>
+      <c r="J24" s="32">
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.45" right="0.2" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCEC0D8-83BC-044E-B61E-C6C5B354CC1E}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1398,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="10">
-        <v>-7.88</v>
+        <v>-0.97460000000000002</v>
       </c>
       <c r="C2" s="11">
         <v>-1.41</v>
@@ -1427,7 +1874,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="12">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="C3" s="13">
         <v>0.15</v>
@@ -1456,7 +1903,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="12">
-        <v>0.47</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C4" s="11">
         <v>-0.15</v>
@@ -1483,10 +1930,10 @@
     </row>
     <row r="5" spans="1:26" ht="40" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B5" s="12">
-        <v>0.44</v>
+        <v>0.37</v>
       </c>
       <c r="C5" s="11">
         <v>-0.1</v>
@@ -1512,10 +1959,10 @@
     </row>
     <row r="6" spans="1:26" ht="40" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="12">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="C6" s="13">
         <v>0.16</v>
@@ -1541,7 +1988,7 @@
     </row>
     <row r="7" spans="1:26" ht="40" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="15">
         <v>0.8</v>
@@ -1577,10 +2024,10 @@
     </row>
     <row r="8" spans="1:26" ht="40" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="18">
-        <v>0.68</v>
+        <v>0.78</v>
       </c>
       <c r="C8" s="16">
         <v>0.8</v>
@@ -1612,16 +2059,15 @@
     </row>
     <row r="9" spans="1:26" ht="49" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="19">
-        <f>C18</f>
-        <v>0.40933333333333333</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="23">
-        <v>0.68</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -1636,7 +2082,7 @@
     </row>
     <row r="10" spans="1:26" ht="53" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
@@ -1654,7 +2100,7 @@
     </row>
     <row r="11" spans="1:26" ht="40" customHeight="1">
       <c r="O11" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
@@ -1674,15 +2120,15 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="O12" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P12" s="26"/>
       <c r="Q12" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R12" s="31"/>
       <c r="S12" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T12" s="27"/>
       <c r="U12" s="27"/>
@@ -1767,7 +2213,7 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="O16" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P16" s="27"/>
       <c r="Q16" s="27">
@@ -1803,7 +2249,7 @@
     <row r="19" spans="1:22" ht="30" customHeight="1">
       <c r="A19" s="1"/>
       <c r="O19" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P19" s="26"/>
       <c r="Q19" s="26"/>
@@ -1816,15 +2262,15 @@
     <row r="20" spans="1:22" ht="24">
       <c r="A20" s="1"/>
       <c r="O20" s="29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P20" s="26"/>
       <c r="Q20" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R20" s="31"/>
       <c r="S20" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T20" s="27"/>
       <c r="U20" s="27"/>
@@ -1878,7 +2324,7 @@
     <row r="24" spans="1:22">
       <c r="A24" s="1"/>
       <c r="O24" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P24" s="27"/>
       <c r="Q24" s="27">

</xml_diff>

<commit_message>
tries to remove cached files
</commit_message>
<xml_diff>
--- a/directors.xlsx
+++ b/directors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshuamailman/Desktop/Metis_Bootcamp/Metis_Bootcamp_repos/scrape_flix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13A5476-4D9C-C147-97B7-00535A7DDC9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE35F2F1-CBB8-3240-9C71-1BC362A7BE5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="460" windowWidth="23680" windowHeight="13920" activeTab="1" xr2:uid="{430FB6C8-4E99-2C4C-88D9-584E09F63679}"/>
+    <workbookView xWindow="6540" yWindow="460" windowWidth="23680" windowHeight="13920" activeTab="2" xr2:uid="{430FB6C8-4E99-2C4C-88D9-584E09F63679}"/>
   </bookViews>
   <sheets>
     <sheet name="poly" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet1!$A$1:$I$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet1!$O$10:$W$25</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -620,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -732,6 +732,9 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3D6B10-E7B3-9142-A566-3C95F796046B}">
   <dimension ref="A10:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -1799,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCEC0D8-83BC-044E-B61E-C6C5B354CC1E}">
   <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2094,11 +2097,13 @@
       <c r="I10" s="22">
         <v>0.69</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" s="55" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="40" customHeight="1">
+      <c r="R10" s="55"/>
+      <c r="S10" s="55"/>
+    </row>
+    <row r="11" spans="1:26" ht="35" customHeight="1">
       <c r="O11" s="29" t="s">
         <v>18</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>20</v>
       </c>
       <c r="P16" s="27"/>
-      <c r="Q16" s="27">
+      <c r="Q16" s="41">
         <f>_xlfn.STDEV.S(Q13:Q15)</f>
         <v>179.75432074454659</v>
       </c>
@@ -2224,7 +2229,7 @@
         <f t="shared" ref="R16" si="2">_xlfn.STDEV.S(R13:R15)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S16" s="27">
+      <c r="S16" s="41">
         <f t="shared" ref="S16" si="3">_xlfn.STDEV.S(S13:S15)</f>
         <v>9.9874921777190956E-2</v>
       </c>
@@ -2242,11 +2247,13 @@
         <f>AVERAGE(B14:C16)</f>
         <v>0.40933333333333333</v>
       </c>
-      <c r="O18" t="s">
+      <c r="Q18" s="55" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="30" customHeight="1">
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+    </row>
+    <row r="19" spans="1:22" ht="35" customHeight="1">
       <c r="A19" s="1"/>
       <c r="O19" s="29" t="s">
         <v>18</v>
@@ -2259,7 +2266,7 @@
       <c r="U19" s="27"/>
       <c r="V19" s="27"/>
     </row>
-    <row r="20" spans="1:22" ht="24">
+    <row r="20" spans="1:22" ht="30" customHeight="1">
       <c r="A20" s="1"/>
       <c r="O20" s="29" t="s">
         <v>19</v>
@@ -2276,7 +2283,7 @@
       <c r="U20" s="27"/>
       <c r="V20" s="27"/>
     </row>
-    <row r="21" spans="1:22" ht="24">
+    <row r="21" spans="1:22" ht="30" customHeight="1">
       <c r="A21" s="1"/>
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
@@ -2291,7 +2298,7 @@
       <c r="U21" s="27"/>
       <c r="V21" s="27"/>
     </row>
-    <row r="22" spans="1:22" ht="24">
+    <row r="22" spans="1:22" ht="30" customHeight="1">
       <c r="A22" s="1"/>
       <c r="O22" s="26"/>
       <c r="P22" s="26"/>
@@ -2306,7 +2313,7 @@
       <c r="U22" s="27"/>
       <c r="V22" s="27"/>
     </row>
-    <row r="23" spans="1:22" ht="24">
+    <row r="23" spans="1:22" ht="30" customHeight="1">
       <c r="A23" s="1"/>
       <c r="O23" s="26"/>
       <c r="P23" s="26"/>
@@ -2321,13 +2328,13 @@
       <c r="U23" s="27"/>
       <c r="V23" s="27"/>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" ht="30" customHeight="1">
       <c r="A24" s="1"/>
       <c r="O24" s="27" t="s">
         <v>20</v>
       </c>
       <c r="P24" s="27"/>
-      <c r="Q24" s="27">
+      <c r="Q24" s="41">
         <f>_xlfn.STDEV.S(Q21:Q23)</f>
         <v>0.41850806443842864</v>
       </c>
@@ -2335,8 +2342,8 @@
         <f t="shared" ref="R24:S24" si="4">_xlfn.STDEV.S(R21:R23)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S24" s="27">
-        <f t="shared" si="4"/>
+      <c r="S24" s="41">
+        <f>_xlfn.STDEV.S(S21:S23)</f>
         <v>8.4689629432022767E-2</v>
       </c>
       <c r="T24" s="27"/>
@@ -2347,6 +2354,10 @@
       <c r="A25" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="Q10:S10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>